<commit_message>
* update 费用报销台账.xlsx * add some new templates * add python-docx to requirements
</commit_message>
<xml_diff>
--- a/templates/费用报销台账.xlsx
+++ b/templates/费用报销台账.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_Project\AutoReimburse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1115F938-3168-4554-8393-A4577F78A2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC08945-4394-431B-9064-3A9F14229732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,7 +167,7 @@
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
     <numFmt numFmtId="178" formatCode="0_ "/>
-    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="179" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -318,6 +318,9 @@
     <xf numFmtId="178" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -332,9 +335,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" x14ac:dyDescent="0.4"/>
@@ -669,16 +669,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.15" x14ac:dyDescent="0.4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="3"/>
@@ -715,7 +715,7 @@
     </row>
     <row r="4" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="17"/>
-      <c r="B4" s="26"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="10"/>
       <c r="D4" s="9"/>
       <c r="E4" s="19"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="5" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="17"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="11"/>
       <c r="D5" s="9"/>
       <c r="E5" s="19"/>
@@ -735,7 +735,7 @@
     </row>
     <row r="6" spans="1:8" ht="31.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="17"/>
-      <c r="B6" s="26"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="11"/>
       <c r="D6" s="9"/>
       <c r="E6" s="19"/>
@@ -745,7 +745,7 @@
     </row>
     <row r="7" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="17"/>
-      <c r="B7" s="26"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="11"/>
       <c r="D7" s="9"/>
       <c r="E7" s="19"/>
@@ -755,7 +755,7 @@
     </row>
     <row r="8" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="17"/>
-      <c r="B8" s="26"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="10"/>
       <c r="D8" s="9"/>
       <c r="E8" s="19"/>
@@ -765,7 +765,7 @@
     </row>
     <row r="9" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="17"/>
-      <c r="B9" s="26"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="10"/>
       <c r="D9" s="9"/>
       <c r="E9" s="19"/>
@@ -775,7 +775,7 @@
     </row>
     <row r="10" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="17"/>
-      <c r="B10" s="26"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="10"/>
       <c r="D10" s="9"/>
       <c r="E10" s="19"/>
@@ -785,7 +785,7 @@
     </row>
     <row r="11" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="17"/>
-      <c r="B11" s="26"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="10"/>
       <c r="D11" s="9"/>
       <c r="E11" s="20"/>
@@ -795,7 +795,7 @@
     </row>
     <row r="12" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="17"/>
-      <c r="B12" s="26"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="10"/>
       <c r="D12" s="9"/>
       <c r="E12" s="20"/>
@@ -805,7 +805,7 @@
     </row>
     <row r="13" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="17"/>
-      <c r="B13" s="26"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="10"/>
       <c r="D13" s="9"/>
       <c r="E13" s="20"/>
@@ -815,7 +815,7 @@
     </row>
     <row r="14" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="17"/>
-      <c r="B14" s="26"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="10"/>
       <c r="D14" s="9"/>
       <c r="E14" s="20"/>
@@ -825,7 +825,7 @@
     </row>
     <row r="15" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="17"/>
-      <c r="B15" s="26"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="11"/>
       <c r="D15" s="9"/>
       <c r="E15" s="20"/>
@@ -834,13 +834,13 @@
       <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="24"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="12" t="str">
-        <f>NUMBERSTRING(F16,2)</f>
-        <v>零</v>
+        <f>TEXT(TRUNC(F16),"[DBNum2]")&amp;"元"&amp;TEXT(RIGHT(FIXED(F16),2),"[dbnum2]0角0分;;"&amp;IF(ABS(F16)&gt;1%,"",))</f>
+        <v>零元</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -857,10 +857,10 @@
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:5" ht="28.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="25"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14" t="s">

</xml_diff>